<commit_message>
Log Book hari ke Tiga
</commit_message>
<xml_diff>
--- a/BurnDownChart_NoWayOut.xlsx
+++ b/BurnDownChart_NoWayOut.xlsx
@@ -63,9 +63,6 @@
     <t>Perubahan iklim dan gaya hidup</t>
   </si>
   <si>
-    <t>Cara Menghemat Listrik</t>
-  </si>
-  <si>
     <t>cara Menghitung Tagihan Listrik</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
   </si>
   <si>
     <t>Apa itu Earth Hour</t>
+  </si>
+  <si>
+    <t>Kenapa Menghemat Listrik?</t>
   </si>
 </sst>
 </file>
@@ -276,36 +276,36 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -598,8 +598,8 @@
   </sheetPr>
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,14 +669,14 @@
       <c r="S2" s="2"/>
     </row>
     <row r="3" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1">
         <v>2</v>
@@ -697,8 +697,8 @@
       <c r="R3" s="1"/>
     </row>
     <row r="4" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="16"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
@@ -721,8 +721,8 @@
       <c r="R4" s="1"/>
     </row>
     <row r="5" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="16"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
@@ -745,8 +745,8 @@
       <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="16"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
@@ -769,10 +769,10 @@
       <c r="R6" s="1"/>
     </row>
     <row r="7" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="16"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D7" s="1">
         <v>5</v>
@@ -793,10 +793,10 @@
       <c r="R7" s="1"/>
     </row>
     <row r="8" spans="1:19" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="17"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="9">
         <v>5</v>
@@ -839,14 +839,14 @@
       <c r="R9" s="10"/>
     </row>
     <row r="10" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D10" s="1">
         <v>4</v>
@@ -867,10 +867,10 @@
       <c r="R10" s="1"/>
     </row>
     <row r="11" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="21"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="1">
         <v>3</v>
@@ -891,10 +891,10 @@
       <c r="R11" s="1"/>
     </row>
     <row r="12" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="21"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1">
         <v>4</v>
@@ -915,10 +915,10 @@
       <c r="R12" s="1"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="21"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="1">
         <v>4</v>
@@ -939,10 +939,10 @@
       <c r="R13" s="1"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="22"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" s="1">
         <v>7</v>
@@ -983,12 +983,12 @@
       <c r="R15" s="11"/>
     </row>
     <row r="16" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="15"/>
+      <c r="B16" s="14"/>
       <c r="C16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" s="1">
         <v>5</v>
@@ -1009,10 +1009,10 @@
       <c r="R16" s="1"/>
     </row>
     <row r="17" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="16"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="15"/>
       <c r="C17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" s="1">
         <v>5</v>
@@ -1033,10 +1033,10 @@
       <c r="R17" s="1"/>
     </row>
     <row r="18" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="17"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D18" s="1">
         <v>5</v>
@@ -1077,12 +1077,12 @@
       <c r="R19" s="12"/>
     </row>
     <row r="20" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="18"/>
+      <c r="B20" s="21"/>
       <c r="C20" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D20" s="1">
         <v>10</v>
@@ -1103,10 +1103,10 @@
       <c r="R20" s="1"/>
     </row>
     <row r="21" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="19"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="22"/>
       <c r="C21" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" s="1">
         <v>10</v>
@@ -1127,11 +1127,11 @@
       <c r="R21" s="1"/>
     </row>
     <row r="22" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
+      <c r="A22" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
       <c r="D22" s="1">
         <f>SUM(D3:D21)</f>
         <v>82</v>
@@ -1194,11 +1194,11 @@
       </c>
     </row>
     <row r="23" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
+      <c r="A23" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
       <c r="D23" s="1">
         <f>SUM(D3:D21)</f>
         <v>82</v>

</xml_diff>